<commit_message>
Most of 7Repl Data From Azure
</commit_message>
<xml_diff>
--- a/docs/data5repl.xlsx
+++ b/docs/data5repl.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\USERDATA\DistSys\chevrotain\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\USERDATA\chevrotain\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A2C994-9FFC-4A22-9FC5-DB4FA56B13F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB1999D-684F-481F-9084-9F99D485A7E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{A478AC17-B821-49E0-BBE5-2534ACF29465}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{A478AC17-B821-49E0-BBE5-2534ACF29465}"/>
   </bookViews>
   <sheets>
     <sheet name="CvRDT-Y" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="13">
   <si>
     <t>10 ops/s</t>
   </si>
@@ -1767,7 +1767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66DAC9F2-CF17-40D5-B51E-826B3CE40E13}">
   <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1796,170 +1796,170 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>422.80694999999997</v>
+        <v>414.49747000000002</v>
       </c>
       <c r="B2">
         <v>100</v>
       </c>
       <c r="D2">
-        <v>421.89478000000003</v>
+        <v>415.697</v>
       </c>
       <c r="E2">
         <v>100</v>
       </c>
       <c r="G2">
-        <v>419.89299999999997</v>
+        <v>415.92944</v>
       </c>
       <c r="H2">
         <v>100</v>
       </c>
       <c r="J2">
-        <v>3181.3289</v>
+        <v>420.04953</v>
       </c>
       <c r="K2">
-        <v>91.646773999999994</v>
+        <v>100</v>
       </c>
       <c r="M2">
-        <v>4727.6977999999999</v>
+        <v>419.67865</v>
       </c>
       <c r="N2">
-        <v>91.217185999999998</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>422.85329999999999</v>
+        <v>420.72370000000001</v>
       </c>
       <c r="B3">
         <v>100</v>
       </c>
       <c r="D3">
-        <v>419.84134</v>
+        <v>415.40260000000001</v>
       </c>
       <c r="E3">
         <v>100</v>
       </c>
       <c r="G3">
-        <v>454.13785000000001</v>
+        <v>419.36856</v>
       </c>
       <c r="H3">
         <v>100</v>
       </c>
       <c r="J3">
-        <v>3918.4011</v>
+        <v>419.19810000000001</v>
       </c>
       <c r="K3">
-        <v>99.856800000000007</v>
+        <v>100</v>
       </c>
       <c r="M3">
-        <v>6372.7334000000001</v>
+        <v>421.07190000000003</v>
       </c>
       <c r="N3">
-        <v>86.634839999999997</v>
+        <v>100</v>
       </c>
       <c r="S3" s="2"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>424.01324</v>
+        <v>418.56738000000001</v>
       </c>
       <c r="B4">
         <v>100</v>
       </c>
       <c r="D4">
-        <v>421.0462</v>
+        <v>413.41025000000002</v>
       </c>
       <c r="E4">
         <v>100</v>
       </c>
       <c r="G4">
-        <v>451.92162999999999</v>
+        <v>422.04903999999999</v>
       </c>
       <c r="H4">
         <v>100</v>
       </c>
       <c r="J4">
-        <v>2455.7024000000001</v>
+        <v>418.08562999999998</v>
       </c>
       <c r="K4">
         <v>100</v>
       </c>
       <c r="M4">
-        <v>6723.9690000000001</v>
+        <v>419.2792</v>
       </c>
       <c r="N4">
-        <v>75.489260000000002</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>420.03183000000001</v>
+        <v>419.78960000000001</v>
       </c>
       <c r="B5">
         <v>100</v>
       </c>
       <c r="D5">
-        <v>417.87643000000003</v>
+        <v>413.37759999999997</v>
       </c>
       <c r="E5">
         <v>100</v>
       </c>
       <c r="G5">
-        <v>423.65404999999998</v>
+        <v>414.77071999999998</v>
       </c>
       <c r="H5">
         <v>100</v>
       </c>
       <c r="J5">
-        <v>4531.5159999999996</v>
+        <v>420.42376999999999</v>
       </c>
       <c r="K5">
         <v>100</v>
       </c>
       <c r="M5">
-        <v>6069.1333000000004</v>
+        <v>422.92325</v>
       </c>
       <c r="N5">
-        <v>92.386634999999998</v>
+        <v>100</v>
       </c>
       <c r="S5" s="1"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>415.11057</v>
+        <v>419.80450000000002</v>
       </c>
       <c r="B6">
         <v>100</v>
       </c>
       <c r="D6">
-        <v>419.45026000000001</v>
+        <v>417.11914000000002</v>
       </c>
       <c r="E6">
         <v>100</v>
       </c>
       <c r="G6">
-        <v>419.96071999999998</v>
+        <v>418.9092</v>
       </c>
       <c r="H6">
         <v>100</v>
       </c>
       <c r="J6">
-        <v>4748.6360000000004</v>
+        <v>418.86383000000001</v>
       </c>
       <c r="K6">
-        <v>96.873509999999996</v>
+        <v>100</v>
       </c>
       <c r="M6">
-        <v>5615.0825000000004</v>
+        <v>415.81610000000001</v>
       </c>
       <c r="N6">
-        <v>88.591880000000003</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f>AVERAGE(A2:A6)</f>
-        <v>420.96317799999997</v>
+        <v>418.67653000000001</v>
       </c>
       <c r="B7" s="1">
         <f>AVERAGE(B2:B6)</f>
@@ -1967,7 +1967,7 @@
       </c>
       <c r="D7" s="1">
         <f>AVERAGE(D2:D6)</f>
-        <v>420.02180200000004</v>
+        <v>415.00131799999997</v>
       </c>
       <c r="E7" s="1">
         <f>AVERAGE(E2:E6)</f>
@@ -1975,7 +1975,7 @@
       </c>
       <c r="G7" s="1">
         <f>AVERAGE(G2:G6)</f>
-        <v>433.91345000000001</v>
+        <v>418.20539200000002</v>
       </c>
       <c r="H7" s="1">
         <f>AVERAGE(H2:H6)</f>
@@ -1983,93 +1983,150 @@
       </c>
       <c r="J7" s="1">
         <f>AVERAGE(J2:J6)</f>
-        <v>3767.11688</v>
+        <v>419.32417199999998</v>
       </c>
       <c r="K7" s="1">
         <f>AVERAGE(K2:K6)</f>
-        <v>97.675416800000008</v>
+        <v>100</v>
       </c>
       <c r="M7" s="1">
         <f>AVERAGE(M2:M6)</f>
-        <v>5901.7232000000004</v>
+        <v>419.75382000000002</v>
       </c>
       <c r="N7" s="1">
         <f>AVERAGE(N2:N6)</f>
-        <v>86.863960199999994</v>
+        <v>100</v>
       </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>497.55594000000002</v>
+      </c>
+      <c r="B10">
+        <v>99.928399999999996</v>
+      </c>
+      <c r="D10">
+        <v>717.10064999999997</v>
+      </c>
+      <c r="E10">
+        <v>94.463009999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>578.57339999999999</v>
+      </c>
+      <c r="B11">
+        <v>99.642005999999995</v>
+      </c>
+      <c r="D11">
+        <v>930.65374999999995</v>
+      </c>
+      <c r="E11">
+        <v>94.677800000000005</v>
+      </c>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>550.68853999999999</v>
+      </c>
+      <c r="B12">
+        <v>100</v>
+      </c>
+      <c r="D12">
+        <v>1658.4861000000001</v>
+      </c>
+      <c r="E12">
+        <v>88.066826000000006</v>
+      </c>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>585.16876000000002</v>
+      </c>
+      <c r="B13">
+        <v>99.928399999999996</v>
+      </c>
+      <c r="D13">
+        <v>1867.1157000000001</v>
+      </c>
+      <c r="E13">
+        <v>71.837710000000001</v>
+      </c>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>880.65099999999995</v>
+      </c>
+      <c r="B14">
+        <v>94.749404999999996</v>
+      </c>
+      <c r="N14" s="2"/>
+    </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="A15" s="1">
+        <f>AVERAGE(A10:A14)</f>
+        <v>618.52752799999996</v>
+      </c>
+      <c r="B15" s="1">
+        <f>AVERAGE(B10:B14)</f>
+        <v>98.849642199999991</v>
+      </c>
+      <c r="D15" s="1">
+        <f>AVERAGE(D10:D14)</f>
+        <v>1293.33905</v>
+      </c>
+      <c r="E15" s="1">
+        <f>AVERAGE(E10:E14)</f>
+        <v>87.261336499999999</v>
+      </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="M15" s="1"/>
+      <c r="L15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="N17" s="1"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="15:17" x14ac:dyDescent="0.25">
       <c r="Q18" s="2"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N19" s="2"/>
+    <row r="19" spans="15:17" x14ac:dyDescent="0.25">
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N20" s="2"/>
+    <row r="20" spans="15:17" x14ac:dyDescent="0.25">
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N21" s="2"/>
+    <row r="21" spans="15:17" x14ac:dyDescent="0.25">
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N22" s="2"/>
+    <row r="22" spans="15:17" x14ac:dyDescent="0.25">
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="N23" s="1"/>
+    <row r="23" spans="15:17" x14ac:dyDescent="0.25">
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
@@ -2083,7 +2140,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79CE1395-6380-422A-83AF-3E7E185B3F85}">
   <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>

</xml_diff>